<commit_message>
fixed problem in inventory load function
</commit_message>
<xml_diff>
--- a/data-raw/correzione_coke.xlsx
+++ b/data-raw/correzione_coke.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/clccr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{F02F116A-9029-4F58-BB2C-78E2F780C50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94FDDC51-9575-4C0B-979C-28E21E12CFF4}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{F02F116A-9029-4F58-BB2C-78E2F780C50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A843368B-3226-4B01-8455-5C8EA2547265}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09F1682C-9829-495D-ADBA-2C1C3F242AF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="17">
   <si>
     <t>Veicolo</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Coal, hard</t>
   </si>
   <si>
-    <t>TOTALE</t>
-  </si>
-  <si>
-    <t>Costruzione</t>
-  </si>
-  <si>
     <t>Batteria</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>Uso</t>
   </si>
   <si>
-    <t>Upstream</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -87,6 +78,15 @@
   </si>
   <si>
     <t>car_petrol</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Vettore energetico</t>
   </si>
 </sst>
 </file>
@@ -145,6 +145,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15E4A62-D30D-49B0-A7AE-1FEA9BF71425}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A19"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,13 +485,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1.0699999999999999E-2</v>
@@ -502,13 +506,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1.54</v>
@@ -523,29 +527,29 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>70.099999999999994</v>
@@ -560,29 +564,29 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>2.3599999999999999E-2</v>
@@ -597,13 +601,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
       </c>
       <c r="D8">
         <v>1.9800000000000002E-2</v>
@@ -618,13 +622,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>1.55</v>
@@ -639,13 +643,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>4.41</v>
@@ -660,13 +664,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>57.8</v>
@@ -681,45 +685,45 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>1.1299999999999999E-2</v>
@@ -734,13 +738,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>1.51</v>
@@ -755,27 +759,27 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <v>70.099999999999994</v>
@@ -790,27 +794,27 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
         <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
       </c>
       <c r="D19">
         <v>2.23E-2</v>
@@ -820,6 +824,350 @@
       </c>
       <c r="F19">
         <f>E19/D19</f>
+        <v>0.29641255605381167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="E20">
+        <v>2.8800000000000002E-3</v>
+      </c>
+      <c r="F20">
+        <f>E20/D20</f>
+        <v>0.2691588785046729</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1.54</v>
+      </c>
+      <c r="E21">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="F21">
+        <f>E21/D21</f>
+        <v>0.2779220779220779</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="E23">
+        <v>6.92</v>
+      </c>
+      <c r="F23">
+        <f>E23/D23</f>
+        <v>9.8716119828815979E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="E25">
+        <v>6.7299999999999999E-3</v>
+      </c>
+      <c r="F25">
+        <f>E25/D25</f>
+        <v>0.28516949152542376</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3.6800000000000001E-3</v>
+      </c>
+      <c r="F26">
+        <f>E26/D26</f>
+        <v>0.18585858585858586</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1.55</v>
+      </c>
+      <c r="E27">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="F27">
+        <f>E27/D27</f>
+        <v>0.31225806451612903</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>4.41</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="F28">
+        <f>E28/D28</f>
+        <v>9.024943310657596E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>57.8</v>
+      </c>
+      <c r="E29">
+        <v>6.39</v>
+      </c>
+      <c r="F29">
+        <f>E29/D29</f>
+        <v>0.11055363321799308</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3.2100000000000002E-3</v>
+      </c>
+      <c r="F32">
+        <f>E32/D32</f>
+        <v>0.28407079646017702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1.51</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.438</v>
+      </c>
+      <c r="F33">
+        <f>E33/D33</f>
+        <v>0.29006622516556291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="E35">
+        <v>6.92</v>
+      </c>
+      <c r="F35">
+        <f>E35/D35</f>
+        <v>9.8716119828815979E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>2.23E-2</v>
+      </c>
+      <c r="E37">
+        <v>6.6100000000000004E-3</v>
+      </c>
+      <c r="F37">
+        <f>E37/D37</f>
         <v>0.29641255605381167</v>
       </c>
     </row>

</xml_diff>